<commit_message>
update - pair programming pre-processing
</commit_message>
<xml_diff>
--- a/external/CelldynParams.xlsx
+++ b/external/CelldynParams.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\laupodteam\AIOS\Bram\notebooks\code_dev\celldyn_embedder\external\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A245E3-2C16-430A-90F0-EED93D363CF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="23625" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Parameters" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Uitleg kleur" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Parameters" sheetId="1" r:id="rId1"/>
+    <sheet name="Uitleg kleur" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -21,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author> </author>
+    <author/>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -36,14 +41,14 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">[Threaded comment]
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Bron: EFLM database</t>
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -53,7 +58,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">[Threaded comment]
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Klinisch/Theoretisch mogelijke waarden. Hierboven of onder is reden voor alertheid. Dit zijn nadrukkelijk GEEN normaalwaarden.</t>
@@ -65,697 +70,694 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="221">
-  <si>
-    <t xml:space="preserve">Naam parameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biologische variatie (%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plausibiliteit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Opmerkingen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eenheid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_wbc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">White Blood Cell Count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*10^9/L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_wvf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">White cell viability fraction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_neu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">neutrofielen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_seg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">segmenten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">De meest mature vorm van de neutrofiel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_bnd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">staven</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_ig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">immature granulocyten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_lym</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lymfocyten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Met name chronische lymfatische leukemieen kunnen zéér hoge aantallen 'normale' lymfocyten tot gevolg hebben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_lyme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_vlym</t>
-  </si>
-  <si>
-    <t xml:space="preserve">absolute concentratie atypische
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="221">
+  <si>
+    <t>Naam parameter</t>
+  </si>
+  <si>
+    <t>Biologische variatie (%)</t>
+  </si>
+  <si>
+    <t>Plausibiliteit</t>
+  </si>
+  <si>
+    <t>Opmerkingen</t>
+  </si>
+  <si>
+    <t>Intra</t>
+  </si>
+  <si>
+    <t>Inter</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Eenheid</t>
+  </si>
+  <si>
+    <t>c_b_wbc</t>
+  </si>
+  <si>
+    <t>White Blood Cell Count</t>
+  </si>
+  <si>
+    <t>10.8</t>
+  </si>
+  <si>
+    <t>16.4</t>
+  </si>
+  <si>
+    <t>*10^9/L</t>
+  </si>
+  <si>
+    <t>c_b_wvf</t>
+  </si>
+  <si>
+    <t>White cell viability fraction</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>c_b_neu</t>
+  </si>
+  <si>
+    <t>neutrofielen</t>
+  </si>
+  <si>
+    <t>14.0</t>
+  </si>
+  <si>
+    <t>23.6</t>
+  </si>
+  <si>
+    <t>c_b_seg</t>
+  </si>
+  <si>
+    <t>segmenten</t>
+  </si>
+  <si>
+    <t>De meest mature vorm van de neutrofiel</t>
+  </si>
+  <si>
+    <t>c_b_bnd</t>
+  </si>
+  <si>
+    <t>staven</t>
+  </si>
+  <si>
+    <t>c_b_ig</t>
+  </si>
+  <si>
+    <t>immature granulocyten</t>
+  </si>
+  <si>
+    <t>c_b_lym</t>
+  </si>
+  <si>
+    <t>lymfocyten</t>
+  </si>
+  <si>
+    <t>22.7</t>
+  </si>
+  <si>
+    <t>Met name chronische lymfatische leukemieen kunnen zéér hoge aantallen 'normale' lymfocyten tot gevolg hebben</t>
+  </si>
+  <si>
+    <t>c_b_lyme</t>
+  </si>
+  <si>
+    <t>c_b_vlym</t>
+  </si>
+  <si>
+    <t>absolute concentratie atypische
 lymfocyten</t>
   </si>
   <si>
-    <t xml:space="preserve">Atypische lymfocyten worden gezien bij infecties of maligniteiten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_mon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">monocyten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_mone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abs conc monocyten als
+    <t>Atypische lymfocyten worden gezien bij infecties of maligniteiten</t>
+  </si>
+  <si>
+    <t>c_b_mon</t>
+  </si>
+  <si>
+    <t>monocyten</t>
+  </si>
+  <si>
+    <t>13.3</t>
+  </si>
+  <si>
+    <t>22.2</t>
+  </si>
+  <si>
+    <t>c_b_mone</t>
+  </si>
+  <si>
+    <t>abs conc monocyten als
 opgesplitst in mon en blast</t>
   </si>
   <si>
-    <t xml:space="preserve">c_b_blst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">absolute concentratie blasten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_eos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eosinofiele granulocyten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_bas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">basofiele granulocyten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_nrbc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">erytroblasten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_pneu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">procentueel aantal neutro's</t>
-  </si>
-  <si>
-    <t xml:space="preserve">%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_pseg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">procentueel aantal segmenten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_pbnd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">procentueel aantal staven</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_pig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">procentueel aantal immature
+    <t>c_b_blst</t>
+  </si>
+  <si>
+    <t>absolute concentratie blasten</t>
+  </si>
+  <si>
+    <t>c_b_eos</t>
+  </si>
+  <si>
+    <t>eosinofiele granulocyten</t>
+  </si>
+  <si>
+    <t>15.0</t>
+  </si>
+  <si>
+    <t>64.4</t>
+  </si>
+  <si>
+    <t>c_b_bas</t>
+  </si>
+  <si>
+    <t>basofiele granulocyten</t>
+  </si>
+  <si>
+    <t>12.4</t>
+  </si>
+  <si>
+    <t>26.3</t>
+  </si>
+  <si>
+    <t>c_b_nrbc</t>
+  </si>
+  <si>
+    <t>erytroblasten</t>
+  </si>
+  <si>
+    <t>c_b_pneu</t>
+  </si>
+  <si>
+    <t>procentueel aantal neutro's</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>c_b_pseg</t>
+  </si>
+  <si>
+    <t>procentueel aantal segmenten</t>
+  </si>
+  <si>
+    <t>c_b_pbnd</t>
+  </si>
+  <si>
+    <t>procentueel aantal staven</t>
+  </si>
+  <si>
+    <t>c_b_pig</t>
+  </si>
+  <si>
+    <t>procentueel aantal immature
 granulocyten</t>
   </si>
   <si>
-    <t xml:space="preserve">c_b_plym</t>
-  </si>
-  <si>
-    <t xml:space="preserve">procentueel aantal lymfocyten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_plyme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">proc conc lymfocyten als
+    <t>c_b_plym</t>
+  </si>
+  <si>
+    <t>procentueel aantal lymfocyten</t>
+  </si>
+  <si>
+    <t>c_b_plyme</t>
+  </si>
+  <si>
+    <t>proc conc lymfocyten als
 opgesplitst in lym en vlym</t>
   </si>
   <si>
-    <t xml:space="preserve">c_b_pvlym</t>
-  </si>
-  <si>
-    <t xml:space="preserve">procentuele concentratie
+    <t>c_b_pvlym</t>
+  </si>
+  <si>
+    <t>procentuele concentratie
 atypische lymfocyten</t>
   </si>
   <si>
-    <t xml:space="preserve">c_b_pmon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">procentueel aantal monocyten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_pmone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">proc conc monocyten als
+    <t>c_b_pmon</t>
+  </si>
+  <si>
+    <t>procentueel aantal monocyten</t>
+  </si>
+  <si>
+    <t>c_b_pmone</t>
+  </si>
+  <si>
+    <t>proc conc monocyten als
 opgesplitst in mon en blasten</t>
   </si>
   <si>
-    <t xml:space="preserve">c_b_pblst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">procentueel aantal blasten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_peos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">procentueel aantal eosinofiele
+    <t>c_b_pblst</t>
+  </si>
+  <si>
+    <t>procentueel aantal blasten</t>
+  </si>
+  <si>
+    <t>c_b_peos</t>
+  </si>
+  <si>
+    <t>procentueel aantal eosinofiele
 granulocyten</t>
   </si>
   <si>
-    <t xml:space="preserve">c_b_pbas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">procentueel aantal basofiele
+    <t>c_b_pbas</t>
+  </si>
+  <si>
+    <t>procentueel aantal basofiele
 granulocyten</t>
   </si>
   <si>
-    <t xml:space="preserve">c_b_pnrbc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">procentueel aantal erytroblasten per 100 WBC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_rbci</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RBC impedantie uitslag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*10^12/L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_rbco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RBC optische uitslag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_hgb_usa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hb uitslag (in USA eenheden)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">g/dL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ik heb in de praktijk een aantal lage Hb metingen gezien. Die patienten waren niet (lang) meer in leven, maar ze waren in principe wel juist.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_mcv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCV uitslag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_rdw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RDW uitslag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_pMIC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">percent of RBCs with volume
+    <t>c_b_pnrbc</t>
+  </si>
+  <si>
+    <t>procentueel aantal erytroblasten per 100 WBC</t>
+  </si>
+  <si>
+    <t>c_b_rbci</t>
+  </si>
+  <si>
+    <t>RBC impedantie uitslag</t>
+  </si>
+  <si>
+    <t>2.6</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>*10^12/L</t>
+  </si>
+  <si>
+    <t>c_b_rbco</t>
+  </si>
+  <si>
+    <t>RBC optische uitslag</t>
+  </si>
+  <si>
+    <t>c_b_hgb_usa</t>
+  </si>
+  <si>
+    <t>Hb uitslag (in USA eenheden)</t>
+  </si>
+  <si>
+    <t>2.7</t>
+  </si>
+  <si>
+    <t>5.9</t>
+  </si>
+  <si>
+    <t>0.8</t>
+  </si>
+  <si>
+    <t>g/dL</t>
+  </si>
+  <si>
+    <t>Ik heb in de praktijk een aantal lage Hb metingen gezien. Die patienten waren niet (lang) meer in leven, maar ze waren in principe wel juist.</t>
+  </si>
+  <si>
+    <t>c_b_mcv</t>
+  </si>
+  <si>
+    <t>MCV uitslag</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
+    <t>fL</t>
+  </si>
+  <si>
+    <t>c_b_rdw</t>
+  </si>
+  <si>
+    <t>RDW uitslag</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>c_b_pMIC</t>
+  </si>
+  <si>
+    <t>percent of RBCs with volume
 less than 60 fL</t>
   </si>
   <si>
-    <t xml:space="preserve">Hemoglobinopathieen kunnen een laag MCV hebben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_pMAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">percent of RBCs with volume
+    <t>Hemoglobinopathieen kunnen een laag MCV hebben</t>
+  </si>
+  <si>
+    <t>c_b_pMAC</t>
+  </si>
+  <si>
+    <t>percent of RBCs with volume
 greater than 120 fL</t>
   </si>
   <si>
-    <t xml:space="preserve">c_b_mch_Usa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCH uitslag (in USA
+    <t>c_b_mch_Usa</t>
+  </si>
+  <si>
+    <t>MCH uitslag (in USA
 eenheden)</t>
   </si>
   <si>
-    <t xml:space="preserve">4.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pg/cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCH = Hb / RBC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_mchc_usa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCHC uitslag (in USA
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>pg/cell</t>
+  </si>
+  <si>
+    <t>MCH = Hb / RBC</t>
+  </si>
+  <si>
+    <t>c_b_mchc_usa</t>
+  </si>
+  <si>
+    <t>MCHC uitslag (in USA
 eenheden)</t>
   </si>
   <si>
-    <t xml:space="preserve">1.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCHC = Hb / Ht</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_ht</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hematocriet uitslag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L/L (%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_plto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLT optische uitslag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_plti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLT impedantie uitslag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_mpv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MPV uitslag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_pct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCT uitslag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_pdw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PDW uitslag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_prP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enumeration of reticulated platelets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_retc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">absoluut aantal reticulocyten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Omgekeerd evenredig met het hemoglobine. Bij een laag Hb verwacht je in gezonde personen een verhoogd aantal reticulocyten. Bij een hoog/normaal Hb verwacht je weinig tot geen reticulocyten. Kunnen afwezig zijnbij aanmaakstoornissen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_pretc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">percentage reticulocyten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_irf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">immature reticulocyte fraction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_pHPO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">percent of RBCs with HGB
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>MCHC = Hb / Ht</t>
+  </si>
+  <si>
+    <t>c_b_ht</t>
+  </si>
+  <si>
+    <t>Hematocriet uitslag</t>
+  </si>
+  <si>
+    <t>2.8</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>L/L (%)</t>
+  </si>
+  <si>
+    <t>PLT</t>
+  </si>
+  <si>
+    <t>c_b_plto</t>
+  </si>
+  <si>
+    <t>PLT optische uitslag</t>
+  </si>
+  <si>
+    <t>7.6</t>
+  </si>
+  <si>
+    <t>18.7</t>
+  </si>
+  <si>
+    <t>c_b_plti</t>
+  </si>
+  <si>
+    <t>PLT impedantie uitslag</t>
+  </si>
+  <si>
+    <t>c_b_mpv</t>
+  </si>
+  <si>
+    <t>MPV uitslag</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>7.1</t>
+  </si>
+  <si>
+    <t>c_b_pct</t>
+  </si>
+  <si>
+    <t>PCT uitslag</t>
+  </si>
+  <si>
+    <t>6.4</t>
+  </si>
+  <si>
+    <t>13.5</t>
+  </si>
+  <si>
+    <t>c_b_pdw</t>
+  </si>
+  <si>
+    <t>PDW uitslag</t>
+  </si>
+  <si>
+    <t>3.8</t>
+  </si>
+  <si>
+    <t>12.3</t>
+  </si>
+  <si>
+    <t>c_b_prP</t>
+  </si>
+  <si>
+    <t>Enumeration of reticulated platelets</t>
+  </si>
+  <si>
+    <t>c_b_retc</t>
+  </si>
+  <si>
+    <t>absoluut aantal reticulocyten</t>
+  </si>
+  <si>
+    <t>9.7</t>
+  </si>
+  <si>
+    <t>27.1</t>
+  </si>
+  <si>
+    <t>Omgekeerd evenredig met het hemoglobine. Bij een laag Hb verwacht je in gezonde personen een verhoogd aantal reticulocyten. Bij een hoog/normaal Hb verwacht je weinig tot geen reticulocyten. Kunnen afwezig zijnbij aanmaakstoornissen.</t>
+  </si>
+  <si>
+    <t>c_b_pretc</t>
+  </si>
+  <si>
+    <t>percentage reticulocyten</t>
+  </si>
+  <si>
+    <t>c_b_irf</t>
+  </si>
+  <si>
+    <t>immature reticulocyte fraction</t>
+  </si>
+  <si>
+    <t>c_b_pHPO</t>
+  </si>
+  <si>
+    <t>percent of RBCs with HGB
 concentration less than 28 g/dL</t>
   </si>
   <si>
-    <t xml:space="preserve">c_b_pHPR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">percent of RBCs with HGB
+    <t>c_b_pHPR</t>
+  </si>
+  <si>
+    <t>percent of RBCs with HGB
 concentration more than 41
 g/dL</t>
   </si>
   <si>
-    <t xml:space="preserve">c_b_HDW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV of the HGB concentration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_MCVr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean volume of reticulocytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_MCHr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean HGB per reticulocyte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_MCHCr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean HGB concentration of reticulocytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_hb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mmol/L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_mch</t>
+    <t>c_b_HDW</t>
+  </si>
+  <si>
+    <t>CV of the HGB concentration</t>
+  </si>
+  <si>
+    <t>c_b_MCVr</t>
+  </si>
+  <si>
+    <t>mean volume of reticulocytes</t>
+  </si>
+  <si>
+    <t>c_b_MCHr</t>
+  </si>
+  <si>
+    <t>mean HGB per reticulocyte</t>
+  </si>
+  <si>
+    <t>c_b_MCHCr</t>
+  </si>
+  <si>
+    <t>mean HGB concentration of reticulocytes</t>
+  </si>
+  <si>
+    <t>c_b_hb</t>
+  </si>
+  <si>
+    <t>mmol/L</t>
+  </si>
+  <si>
+    <t>c_b_mch</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">c_b_mchc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_namn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean neutro's 0 graden (ALL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_nacv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV% neutro's 0 graden (ALL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_nimn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean neutro's 7 graden (IAS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_nicv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV% neutro's 7 graden (IAS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_npmn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean neutro's 90 graden (PSS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_npcv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV% neutro's 90 graden (PSS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_ndmn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean neutro's 90 graden
+    <t>c_b_mchc</t>
+  </si>
+  <si>
+    <t>c_b_namn</t>
+  </si>
+  <si>
+    <t>mean neutro's 0 graden (ALL)</t>
+  </si>
+  <si>
+    <t>c_b_nacv</t>
+  </si>
+  <si>
+    <t>CV% neutro's 0 graden (ALL)</t>
+  </si>
+  <si>
+    <t>c_b_nimn</t>
+  </si>
+  <si>
+    <t>mean neutro's 7 graden (IAS)</t>
+  </si>
+  <si>
+    <t>c_b_nicv</t>
+  </si>
+  <si>
+    <t>CV% neutro's 7 graden (IAS)</t>
+  </si>
+  <si>
+    <t>c_b_npmn</t>
+  </si>
+  <si>
+    <t>mean neutro's 90 graden (PSS)</t>
+  </si>
+  <si>
+    <t>c_b_npcv</t>
+  </si>
+  <si>
+    <t>CV% neutro's 90 graden (PSS)</t>
+  </si>
+  <si>
+    <t>c_b_ndmn</t>
+  </si>
+  <si>
+    <t>mean neutro's 90 graden
 gedepolariseerd (DSS)</t>
   </si>
   <si>
-    <t xml:space="preserve">c_b_ndcv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV% neutro's 90 graden
+    <t>c_b_ndcv</t>
+  </si>
+  <si>
+    <t>CV% neutro's 90 graden
 gedepolariseerd (DSS)</t>
   </si>
   <si>
-    <t xml:space="preserve">c_b_nfmn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean neutro's FL3 kanaal (FL3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_nfcv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV% neutro's FL3 kanaal (FL3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_Lamn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean lymfo's 0 graden (ALL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_Lacv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV% lymfo's 0 graden (ALL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_Limn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean lymfo's 7 graden (IAS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_Licv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV% lymfo's 7 graden (IAS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_Pimn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean trombo's 7 graden (IAS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_Picv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV% trombo's 7 graden (IAS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_Ppmn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean trombo's 90 graden
+    <t>c_b_nfmn</t>
+  </si>
+  <si>
+    <t>mean neutro's FL3 kanaal (FL3)</t>
+  </si>
+  <si>
+    <t>c_b_nfcv</t>
+  </si>
+  <si>
+    <t>CV% neutro's FL3 kanaal (FL3)</t>
+  </si>
+  <si>
+    <t>c_b_Lamn</t>
+  </si>
+  <si>
+    <t>mean lymfo's 0 graden (ALL)</t>
+  </si>
+  <si>
+    <t>c_b_Lacv</t>
+  </si>
+  <si>
+    <t>CV% lymfo's 0 graden (ALL)</t>
+  </si>
+  <si>
+    <t>c_b_Limn</t>
+  </si>
+  <si>
+    <t>mean lymfo's 7 graden (IAS)</t>
+  </si>
+  <si>
+    <t>c_b_Licv</t>
+  </si>
+  <si>
+    <t>CV% lymfo's 7 graden (IAS)</t>
+  </si>
+  <si>
+    <t>c_b_Pimn</t>
+  </si>
+  <si>
+    <t>mean trombo's 7 graden (IAS)</t>
+  </si>
+  <si>
+    <t>c_b_Picv</t>
+  </si>
+  <si>
+    <t>CV% trombo's 7 graden (IAS)</t>
+  </si>
+  <si>
+    <t>c_b_Ppmn</t>
+  </si>
+  <si>
+    <t>mean trombo's 90 graden
 (PSS)</t>
   </si>
   <si>
-    <t xml:space="preserve">c_b_Ppcv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV% trombo's 90 graden (PSS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_rbcimn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean rbc  7 graden (IAS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_rbcicv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV% rbc  7 graden (IAS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_rbcfmn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean rbc  FL3 kanaal (FL3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_b_rbcfcv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV% rbc  FL3 kanaal (FL3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plaatjes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scatter</t>
+    <t>c_b_Ppcv</t>
+  </si>
+  <si>
+    <t>CV% trombo's 90 graden (PSS)</t>
+  </si>
+  <si>
+    <t>c_b_rbcimn</t>
+  </si>
+  <si>
+    <t>mean rbc  7 graden (IAS)</t>
+  </si>
+  <si>
+    <t>c_b_rbcicv</t>
+  </si>
+  <si>
+    <t>CV% rbc  7 graden (IAS)</t>
+  </si>
+  <si>
+    <t>c_b_rbcfmn</t>
+  </si>
+  <si>
+    <t>mean rbc  FL3 kanaal (FL3)</t>
+  </si>
+  <si>
+    <t>c_b_rbcfcv</t>
+  </si>
+  <si>
+    <t>CV% rbc  FL3 kanaal (FL3)</t>
+  </si>
+  <si>
+    <t>Wit</t>
+  </si>
+  <si>
+    <t>Rood</t>
+  </si>
+  <si>
+    <t>Plaatjes</t>
+  </si>
+  <si>
+    <t>Scatter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -764,29 +766,13 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
       <sz val="9.5"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -794,8 +780,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <i val="true"/>
+      <b/>
+      <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -803,7 +789,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="9.5"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -858,14 +844,14 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFC1C1C1"/>
       </left>
@@ -881,134 +867,78 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Standaard 2" xfId="20"/>
+  <cellStyles count="2">
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1067,53 +997,360 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B41" activeCellId="0" sqref="B41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="118.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.14"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="118.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2"/>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1130,7 +1367,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -1143,13 +1380,13 @@
       <c r="D3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="2">
         <v>0</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="2">
         <v>1000</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="8"/>
@@ -1159,7 +1396,7 @@
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
@@ -1172,13 +1409,13 @@
       <c r="D4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H4" s="8"/>
@@ -1188,7 +1425,7 @@
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
@@ -1201,13 +1438,13 @@
       <c r="D5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="2">
         <v>0</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="F5" s="2">
         <v>300</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="8"/>
@@ -1217,7 +1454,7 @@
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
@@ -1230,13 +1467,13 @@
       <c r="D6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="2">
         <v>0</v>
       </c>
-      <c r="F6" s="1" t="n">
+      <c r="F6" s="2">
         <v>300</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H6" s="8" t="s">
@@ -1248,7 +1485,7 @@
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
@@ -1261,13 +1498,13 @@
       <c r="D7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="2">
         <v>0</v>
       </c>
-      <c r="F7" s="1" t="n">
+      <c r="F7" s="2">
         <v>300</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H7" s="8"/>
@@ -1277,7 +1514,7 @@
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>26</v>
       </c>
@@ -1290,13 +1527,13 @@
       <c r="D8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="2">
         <v>0</v>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="F8" s="2">
         <v>300</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H8" s="8"/>
@@ -1306,7 +1543,7 @@
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
@@ -1319,13 +1556,13 @@
       <c r="D9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="2">
         <v>0</v>
       </c>
-      <c r="F9" s="1" t="n">
+      <c r="F9" s="2">
         <v>1000</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="8" t="s">
@@ -1337,7 +1574,7 @@
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
@@ -1350,13 +1587,13 @@
       <c r="D10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="E10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H10" s="8"/>
@@ -1366,7 +1603,7 @@
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>33</v>
       </c>
@@ -1379,13 +1616,13 @@
       <c r="D11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="2">
         <v>0</v>
       </c>
-      <c r="F11" s="1" t="n">
+      <c r="F11" s="2">
         <v>1000</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="8" t="s">
@@ -1397,7 +1634,7 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -1410,13 +1647,13 @@
       <c r="D12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="2">
         <v>0</v>
       </c>
-      <c r="F12" s="1" t="n">
+      <c r="F12" s="2">
         <v>300</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="8"/>
@@ -1426,7 +1663,7 @@
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>40</v>
       </c>
@@ -1439,13 +1676,13 @@
       <c r="D13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="1" t="s">
+      <c r="E13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H13" s="8"/>
@@ -1455,7 +1692,7 @@
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>42</v>
       </c>
@@ -1468,13 +1705,13 @@
       <c r="D14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="2">
         <v>0</v>
       </c>
-      <c r="F14" s="1" t="n">
+      <c r="F14" s="2">
         <v>1000</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H14" s="8"/>
@@ -1484,7 +1721,7 @@
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>44</v>
       </c>
@@ -1497,13 +1734,13 @@
       <c r="D15" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="2">
         <v>0</v>
       </c>
-      <c r="F15" s="1" t="n">
+      <c r="F15" s="2">
         <v>100</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H15" s="8"/>
@@ -1513,7 +1750,7 @@
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>48</v>
       </c>
@@ -1526,13 +1763,13 @@
       <c r="D16" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="1" t="n">
+      <c r="E16" s="2">
         <v>0</v>
       </c>
-      <c r="F16" s="1" t="n">
+      <c r="F16" s="2">
         <v>100</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H16" s="8"/>
@@ -1542,7 +1779,7 @@
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>52</v>
       </c>
@@ -1555,13 +1792,13 @@
       <c r="D17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="1" t="n">
+      <c r="E17" s="2">
         <v>0</v>
       </c>
-      <c r="F17" s="1" t="n">
+      <c r="F17" s="2">
         <v>50</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H17" s="8"/>
@@ -1571,7 +1808,7 @@
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>54</v>
       </c>
@@ -1584,13 +1821,13 @@
       <c r="D18" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="1" t="n">
+      <c r="E18" s="2">
         <v>0</v>
       </c>
-      <c r="F18" s="1" t="n">
+      <c r="F18" s="2">
         <v>100</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="2" t="s">
         <v>56</v>
       </c>
       <c r="H18" s="8"/>
@@ -1600,7 +1837,7 @@
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>57</v>
       </c>
@@ -1613,13 +1850,13 @@
       <c r="D19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="E19" s="2">
         <v>0</v>
       </c>
-      <c r="F19" s="1" t="n">
+      <c r="F19" s="2">
         <v>100</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="2" t="s">
         <v>56</v>
       </c>
       <c r="H19" s="8"/>
@@ -1629,7 +1866,7 @@
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>59</v>
       </c>
@@ -1642,13 +1879,13 @@
       <c r="D20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="1" t="n">
+      <c r="E20" s="2">
         <v>0</v>
       </c>
-      <c r="F20" s="1" t="n">
+      <c r="F20" s="2">
         <v>100</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="2" t="s">
         <v>56</v>
       </c>
       <c r="H20" s="8"/>
@@ -1658,7 +1895,7 @@
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>61</v>
       </c>
@@ -1671,13 +1908,13 @@
       <c r="D21" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="1" t="n">
+      <c r="E21" s="2">
         <v>0</v>
       </c>
-      <c r="F21" s="1" t="n">
+      <c r="F21" s="2">
         <v>100</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="2" t="s">
         <v>56</v>
       </c>
       <c r="H21" s="8"/>
@@ -1687,7 +1924,7 @@
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>63</v>
       </c>
@@ -1700,13 +1937,13 @@
       <c r="D22" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="1" t="n">
+      <c r="E22" s="2">
         <v>0</v>
       </c>
-      <c r="F22" s="1" t="n">
+      <c r="F22" s="2">
         <v>100</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="2" t="s">
         <v>56</v>
       </c>
       <c r="H22" s="8"/>
@@ -1716,7 +1953,7 @@
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>65</v>
       </c>
@@ -1729,13 +1966,13 @@
       <c r="D23" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G23" s="1" t="s">
+      <c r="E23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H23" s="8"/>
@@ -1745,7 +1982,7 @@
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>67</v>
       </c>
@@ -1758,13 +1995,13 @@
       <c r="D24" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="1" t="n">
+      <c r="E24" s="2">
         <v>0</v>
       </c>
-      <c r="F24" s="1" t="n">
+      <c r="F24" s="2">
         <v>100</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" s="2" t="s">
         <v>56</v>
       </c>
       <c r="H24" s="8"/>
@@ -1774,7 +2011,7 @@
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>69</v>
       </c>
@@ -1787,13 +2024,13 @@
       <c r="D25" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="1" t="n">
+      <c r="E25" s="2">
         <v>0</v>
       </c>
-      <c r="F25" s="1" t="n">
+      <c r="F25" s="2">
         <v>60</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="2" t="s">
         <v>56</v>
       </c>
       <c r="H25" s="8"/>
@@ -1803,7 +2040,7 @@
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>71</v>
       </c>
@@ -1816,13 +2053,13 @@
       <c r="D26" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="1" t="s">
+      <c r="E26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H26" s="8"/>
@@ -1832,7 +2069,7 @@
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>73</v>
       </c>
@@ -1845,13 +2082,13 @@
       <c r="D27" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="1" t="n">
+      <c r="E27" s="2">
         <v>0</v>
       </c>
-      <c r="F27" s="1" t="n">
+      <c r="F27" s="2">
         <v>100</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G27" s="2" t="s">
         <v>56</v>
       </c>
       <c r="H27" s="8"/>
@@ -1861,7 +2098,7 @@
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>75</v>
       </c>
@@ -1874,13 +2111,13 @@
       <c r="D28" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="1" t="n">
+      <c r="E28" s="2">
         <v>0</v>
       </c>
-      <c r="F28" s="1" t="n">
+      <c r="F28" s="2">
         <v>80</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="2" t="s">
         <v>56</v>
       </c>
       <c r="H28" s="8"/>
@@ -1890,7 +2127,7 @@
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>77</v>
       </c>
@@ -1903,13 +2140,13 @@
       <c r="D29" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="1" t="n">
+      <c r="E29" s="2">
         <v>0</v>
       </c>
-      <c r="F29" s="1" t="n">
+      <c r="F29" s="2">
         <v>80</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" s="2" t="s">
         <v>56</v>
       </c>
       <c r="H29" s="8"/>
@@ -1919,7 +2156,7 @@
       <c r="L29" s="8"/>
       <c r="M29" s="8"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>79</v>
       </c>
@@ -1932,10 +2169,10 @@
       <c r="D30" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E30" s="7" t="n">
+      <c r="E30" s="7">
         <v>0</v>
       </c>
-      <c r="F30" s="7" t="n">
+      <c r="F30" s="7">
         <v>80</v>
       </c>
       <c r="G30" s="7" t="s">
@@ -1948,7 +2185,7 @@
       <c r="L30" s="8"/>
       <c r="M30" s="8"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>81</v>
       </c>
@@ -1961,13 +2198,13 @@
       <c r="D31" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F31" s="1" t="n">
+      <c r="F31" s="2">
         <v>15</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G31" s="2" t="s">
         <v>86</v>
       </c>
       <c r="H31" s="8"/>
@@ -1977,7 +2214,7 @@
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>87</v>
       </c>
@@ -1990,13 +2227,13 @@
       <c r="D32" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F32" s="1" t="n">
+      <c r="F32" s="2">
         <v>15</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G32" s="2" t="s">
         <v>86</v>
       </c>
       <c r="H32" s="8"/>
@@ -2006,7 +2243,7 @@
       <c r="L32" s="8"/>
       <c r="M32" s="8"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>89</v>
       </c>
@@ -2019,13 +2256,13 @@
       <c r="D33" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F33" s="1" t="n">
+      <c r="F33" s="2">
         <v>25</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G33" s="2" t="s">
         <v>94</v>
       </c>
       <c r="H33" s="8" t="s">
@@ -2037,7 +2274,7 @@
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>96</v>
       </c>
@@ -2050,13 +2287,13 @@
       <c r="D34" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E34" s="1" t="n">
+      <c r="E34" s="2">
         <v>40</v>
       </c>
-      <c r="F34" s="1" t="n">
+      <c r="F34" s="2">
         <v>160</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G34" s="2" t="s">
         <v>99</v>
       </c>
       <c r="H34" s="8"/>
@@ -2066,7 +2303,7 @@
       <c r="L34" s="8"/>
       <c r="M34" s="8"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>100</v>
       </c>
@@ -2079,13 +2316,13 @@
       <c r="D35" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E35" s="1" t="n">
+      <c r="E35" s="2">
         <v>5</v>
       </c>
-      <c r="F35" s="1" t="n">
+      <c r="F35" s="2">
         <v>50</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G35" s="2" t="s">
         <v>56</v>
       </c>
       <c r="H35" s="8"/>
@@ -2095,7 +2332,7 @@
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>104</v>
       </c>
@@ -2108,13 +2345,13 @@
       <c r="D36" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="1" t="n">
+      <c r="E36" s="2">
         <v>0</v>
       </c>
-      <c r="F36" s="1" t="n">
+      <c r="F36" s="2">
         <v>100</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G36" s="2" t="s">
         <v>56</v>
       </c>
       <c r="H36" s="8" t="s">
@@ -2126,7 +2363,7 @@
       <c r="L36" s="8"/>
       <c r="M36" s="8"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>107</v>
       </c>
@@ -2139,13 +2376,13 @@
       <c r="D37" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E37" s="1" t="n">
+      <c r="E37" s="2">
         <v>0</v>
       </c>
-      <c r="F37" s="1" t="n">
+      <c r="F37" s="2">
         <v>100</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G37" s="2" t="s">
         <v>56</v>
       </c>
       <c r="H37" s="8"/>
@@ -2155,7 +2392,7 @@
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>109</v>
       </c>
@@ -2168,13 +2405,13 @@
       <c r="D38" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F38" s="1" t="n">
+      <c r="F38" s="2">
         <v>161</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G38" s="2" t="s">
         <v>113</v>
       </c>
       <c r="H38" s="8" t="s">
@@ -2186,7 +2423,7 @@
       <c r="L38" s="8"/>
       <c r="M38" s="8"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>115</v>
       </c>
@@ -2199,13 +2436,13 @@
       <c r="D39" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E39" s="1" t="n">
+      <c r="E39" s="2">
         <v>0</v>
       </c>
-      <c r="F39" s="1" t="n">
+      <c r="F39" s="2">
         <v>80</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G39" s="2" t="s">
         <v>94</v>
       </c>
       <c r="H39" s="8" t="s">
@@ -2217,7 +2454,7 @@
       <c r="L39" s="8"/>
       <c r="M39" s="8"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>120</v>
       </c>
@@ -2230,13 +2467,13 @@
       <c r="D40" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G40" s="1" t="s">
+      <c r="E40" s="2">
+        <v>20</v>
+      </c>
+      <c r="F40" s="2">
+        <v>80</v>
+      </c>
+      <c r="G40" s="2" t="s">
         <v>125</v>
       </c>
       <c r="H40" s="8"/>
@@ -2246,7 +2483,7 @@
       <c r="L40" s="8"/>
       <c r="M40" s="8"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>126</v>
       </c>
@@ -2262,7 +2499,7 @@
       <c r="L41" s="8"/>
       <c r="M41" s="8"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>127</v>
       </c>
@@ -2275,13 +2512,13 @@
       <c r="D42" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="E42" s="1" t="n">
+      <c r="E42" s="2">
         <v>0</v>
       </c>
-      <c r="F42" s="1" t="n">
+      <c r="F42" s="2">
         <v>2000</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G42" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H42" s="8"/>
@@ -2291,7 +2528,7 @@
       <c r="L42" s="8"/>
       <c r="M42" s="8"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>131</v>
       </c>
@@ -2304,13 +2541,13 @@
       <c r="D43" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="E43" s="1" t="n">
+      <c r="E43" s="2">
         <v>0</v>
       </c>
-      <c r="F43" s="1" t="n">
+      <c r="F43" s="2">
         <v>2000</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G43" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H43" s="8"/>
@@ -2320,7 +2557,7 @@
       <c r="L43" s="8"/>
       <c r="M43" s="8"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>133</v>
       </c>
@@ -2333,10 +2570,10 @@
       <c r="D44" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="E44" s="7" t="n">
+      <c r="E44" s="7">
         <v>1</v>
       </c>
-      <c r="F44" s="7" t="n">
+      <c r="F44" s="7">
         <v>20</v>
       </c>
       <c r="G44" s="7" t="s">
@@ -2349,7 +2586,7 @@
       <c r="L44" s="8"/>
       <c r="M44" s="8"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>137</v>
       </c>
@@ -2378,7 +2615,7 @@
       <c r="L45" s="8"/>
       <c r="M45" s="8"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>141</v>
       </c>
@@ -2407,7 +2644,7 @@
       <c r="L46" s="8"/>
       <c r="M46" s="8"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>145</v>
       </c>
@@ -2436,7 +2673,7 @@
       <c r="L47" s="8"/>
       <c r="M47" s="8"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>147</v>
       </c>
@@ -2449,13 +2686,13 @@
       <c r="D48" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="E48" s="1" t="n">
+      <c r="E48" s="2">
         <v>0</v>
       </c>
-      <c r="F48" s="1" t="n">
+      <c r="F48" s="2">
         <v>600</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="G48" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H48" s="8" t="s">
@@ -2467,7 +2704,7 @@
       <c r="L48" s="8"/>
       <c r="M48" s="8"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>152</v>
       </c>
@@ -2496,7 +2733,7 @@
       <c r="L49" s="8"/>
       <c r="M49" s="8"/>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>154</v>
       </c>
@@ -2525,7 +2762,7 @@
       <c r="L50" s="8"/>
       <c r="M50" s="8"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>156</v>
       </c>
@@ -2554,7 +2791,7 @@
       <c r="L51" s="8"/>
       <c r="M51" s="8"/>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:13" ht="39" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>158</v>
       </c>
@@ -2583,7 +2820,7 @@
       <c r="L52" s="8"/>
       <c r="M52" s="8"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>160</v>
       </c>
@@ -2612,7 +2849,7 @@
       <c r="L53" s="8"/>
       <c r="M53" s="8"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>162</v>
       </c>
@@ -2641,7 +2878,7 @@
       <c r="L54" s="8"/>
       <c r="M54" s="8"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>164</v>
       </c>
@@ -2670,7 +2907,7 @@
       <c r="L55" s="8"/>
       <c r="M55" s="8"/>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>166</v>
       </c>
@@ -2699,7 +2936,7 @@
       <c r="L56" s="8"/>
       <c r="M56" s="8"/>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>168</v>
       </c>
@@ -2713,10 +2950,10 @@
       <c r="E57" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="F57" s="7" t="n">
+      <c r="F57" s="7">
         <v>15</v>
       </c>
-      <c r="G57" s="1" t="s">
+      <c r="G57" s="2" t="s">
         <v>169</v>
       </c>
       <c r="H57" s="8" t="s">
@@ -2728,7 +2965,7 @@
       <c r="L57" s="8"/>
       <c r="M57" s="8"/>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
         <v>170</v>
       </c>
@@ -2741,13 +2978,13 @@
       <c r="D58" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E58" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F58" s="1" t="n">
+      <c r="F58" s="2">
         <v>10</v>
       </c>
-      <c r="G58" s="1" t="s">
+      <c r="G58" s="2" t="s">
         <v>169</v>
       </c>
       <c r="H58" s="8"/>
@@ -2757,7 +2994,7 @@
       <c r="L58" s="8"/>
       <c r="M58" s="8"/>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>172</v>
       </c>
@@ -2770,13 +3007,13 @@
       <c r="D59" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E59" s="1" t="n">
+      <c r="E59" s="2">
         <v>0</v>
       </c>
-      <c r="F59" s="1" t="n">
+      <c r="F59" s="2">
         <v>50</v>
       </c>
-      <c r="G59" s="1" t="s">
+      <c r="G59" s="2" t="s">
         <v>169</v>
       </c>
       <c r="H59" s="8"/>
@@ -2786,7 +3023,7 @@
       <c r="L59" s="8"/>
       <c r="M59" s="8"/>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
         <v>173</v>
       </c>
@@ -2815,7 +3052,7 @@
       <c r="L60" s="8"/>
       <c r="M60" s="8"/>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
         <v>175</v>
       </c>
@@ -2844,7 +3081,7 @@
       <c r="L61" s="8"/>
       <c r="M61" s="8"/>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="18" t="s">
         <v>177</v>
       </c>
@@ -2873,7 +3110,7 @@
       <c r="L62" s="8"/>
       <c r="M62" s="8"/>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
         <v>179</v>
       </c>
@@ -2902,7 +3139,7 @@
       <c r="L63" s="8"/>
       <c r="M63" s="8"/>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
         <v>181</v>
       </c>
@@ -2931,7 +3168,7 @@
       <c r="L64" s="8"/>
       <c r="M64" s="8"/>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
         <v>183</v>
       </c>
@@ -2960,7 +3197,7 @@
       <c r="L65" s="8"/>
       <c r="M65" s="8"/>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A66" s="18" t="s">
         <v>185</v>
       </c>
@@ -2989,7 +3226,7 @@
       <c r="L66" s="8"/>
       <c r="M66" s="8"/>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A67" s="18" t="s">
         <v>187</v>
       </c>
@@ -3018,7 +3255,7 @@
       <c r="L67" s="8"/>
       <c r="M67" s="8"/>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
         <v>189</v>
       </c>
@@ -3047,7 +3284,7 @@
       <c r="L68" s="8"/>
       <c r="M68" s="8"/>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="18" t="s">
         <v>191</v>
       </c>
@@ -3076,7 +3313,7 @@
       <c r="L69" s="8"/>
       <c r="M69" s="8"/>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
         <v>193</v>
       </c>
@@ -3105,7 +3342,7 @@
       <c r="L70" s="8"/>
       <c r="M70" s="8"/>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="18" t="s">
         <v>195</v>
       </c>
@@ -3134,7 +3371,7 @@
       <c r="L71" s="8"/>
       <c r="M71" s="8"/>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
         <v>197</v>
       </c>
@@ -3163,7 +3400,7 @@
       <c r="L72" s="8"/>
       <c r="M72" s="8"/>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="18" t="s">
         <v>199</v>
       </c>
@@ -3192,7 +3429,7 @@
       <c r="L73" s="8"/>
       <c r="M73" s="8"/>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="18" t="s">
         <v>201</v>
       </c>
@@ -3221,7 +3458,7 @@
       <c r="L74" s="8"/>
       <c r="M74" s="8"/>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="18" t="s">
         <v>203</v>
       </c>
@@ -3250,7 +3487,7 @@
       <c r="L75" s="8"/>
       <c r="M75" s="8"/>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
         <v>205</v>
       </c>
@@ -3279,7 +3516,7 @@
       <c r="L76" s="8"/>
       <c r="M76" s="8"/>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
         <v>207</v>
       </c>
@@ -3308,7 +3545,7 @@
       <c r="L77" s="8"/>
       <c r="M77" s="8"/>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="18" t="s">
         <v>209</v>
       </c>
@@ -3337,7 +3574,7 @@
       <c r="L78" s="8"/>
       <c r="M78" s="8"/>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="18" t="s">
         <v>211</v>
       </c>
@@ -3366,7 +3603,7 @@
       <c r="L79" s="8"/>
       <c r="M79" s="8"/>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="18" t="s">
         <v>213</v>
       </c>
@@ -3395,7 +3632,7 @@
       <c r="L80" s="8"/>
       <c r="M80" s="8"/>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="18" t="s">
         <v>215</v>
       </c>
@@ -3429,216 +3666,44 @@
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:G1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>220</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D7617B8D9C0039498B46A476FE5DF18F" ma:contentTypeVersion="2" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="9238698a898bcdf62808e72e90241979">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f672487a-9762-4dd8-8daf-dbc760d273ee" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5a9634a08892653ebbd837227d8a57b8" ns2:_="">
-    <xsd:import namespace="f672487a-9762-4dd8-8daf-dbc760d273ee"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="f672487a-9762-4dd8-8daf-dbc760d273ee" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhoudstype"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DBFAC1B-E8DC-4905-BCA8-DA411070D41F}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1724689-04DB-490C-84CC-57592E574204}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0C27105-1CE0-40F2-B61A-B56B2D2F02DB}"/>
 </file>
</xml_diff>